<commit_message>
add: preview import teacher
</commit_message>
<xml_diff>
--- a/public/init_data/teacher_init.xlsx
+++ b/public/init_data/teacher_init.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HTTT\DoAnTN\Project\FE3\public\init_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88467EDC-9FE1-4369-9057-2E40AA026688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250F8427-ECB9-4A15-8004-79CE20C6F90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{B8962491-F3BD-455F-A1CF-BA3E487930C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>STT</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Thanh Bình</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Thị </t>
   </si>
   <si>
     <t>Xuân Hiền</t>
@@ -533,7 +530,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -690,12 +687,6 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>20012016</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
@@ -714,10 +705,10 @@
         <v>20012017</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>12</v>
@@ -734,10 +725,10 @@
         <v>20012018</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>13</v>
@@ -754,10 +745,10 @@
         <v>20012019</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -774,10 +765,10 @@
         <v>20012020</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>15</v>

</xml_diff>